<commit_message>
Updating requirements.txt using pipreqs
</commit_message>
<xml_diff>
--- a/Data Cleaning Information Storage.xlsx
+++ b/Data Cleaning Information Storage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Semester Name</t>
   </si>
@@ -33,24 +33,30 @@
     <t>Second Semester</t>
   </si>
   <si>
+    <t>Other Semester</t>
+  </si>
+  <si>
     <t>1/11/2011</t>
   </si>
   <si>
     <t>3/2/2024</t>
   </si>
   <si>
+    <t>3/3/2028</t>
+  </si>
+  <si>
     <t>3/1/2024</t>
   </si>
   <si>
     <t>3/2/2028</t>
   </si>
   <si>
+    <t>4/4/2029</t>
+  </si>
+  <si>
     <t>Staff Emails</t>
   </si>
   <si>
-    <t>schwartzd@brandeis.edu</t>
-  </si>
-  <si>
     <t>ldropkin@brandeis.edu</t>
   </si>
   <si>
@@ -63,6 +69,9 @@
     <t>xiaoyizhang@brandeis.edu</t>
   </si>
   <si>
+    <t>jschlesinger@brandeis.edu</t>
+  </si>
+  <si>
     <t>Appointment Type</t>
   </si>
   <si>
@@ -91,6 +100,9 @@
   </si>
   <si>
     <t xml:space="preserve">Club Support </t>
+  </si>
+  <si>
+    <t>Law</t>
   </si>
   <si>
     <t>Appointment</t>
@@ -454,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -476,10 +488,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -487,10 +499,21 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -500,7 +523,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -508,32 +531,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -551,68 +574,74 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to add deletion logs and functionality for combined data cleaning
</commit_message>
<xml_diff>
--- a/Data Cleaning Information Storage.xlsx
+++ b/Data Cleaning Information Storage.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowanscassellati/Documents/GitHub/DSI-Hiatt-Visualizations/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FA1C51-9D43-A442-98D7-B6B5EE6910B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semester Information" sheetId="1" r:id="rId1"/>
     <sheet name="Hiatt Staff Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Appointment Type Summation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Semester Name</t>
   </si>
@@ -27,36 +33,12 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>First Semester</t>
-  </si>
-  <si>
-    <t>Second Semester</t>
-  </si>
-  <si>
-    <t>Other Semester</t>
-  </si>
-  <si>
-    <t>1/11/2011</t>
-  </si>
-  <si>
-    <t>3/2/2024</t>
-  </si>
-  <si>
-    <t>3/3/2028</t>
-  </si>
-  <si>
-    <t>3/1/2024</t>
-  </si>
-  <si>
-    <t>3/2/2028</t>
-  </si>
-  <si>
-    <t>4/4/2029</t>
-  </si>
-  <si>
     <t>Staff Emails</t>
   </si>
   <si>
+    <t>schwartzd@brandeis.edu</t>
+  </si>
+  <si>
     <t>ldropkin@brandeis.edu</t>
   </si>
   <si>
@@ -102,20 +84,17 @@
     <t xml:space="preserve">Club Support </t>
   </si>
   <si>
-    <t>Law</t>
-  </si>
-  <si>
-    <t>Appointment</t>
-  </si>
-  <si>
-    <t>Not Drop In</t>
+    <t>This is a semester name that should get replaced</t>
+  </si>
+  <si>
+    <t>1/1/1111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,24 +146,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -222,7 +210,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -256,6 +244,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -290,9 +279,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,14 +455,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,37 +475,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="C2" s="2">
+        <v>55134</v>
       </c>
     </row>
   </sheetData>
@@ -522,41 +492,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -565,83 +540,61 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Force output for semester to appear as strings
</commit_message>
<xml_diff>
--- a/Data Cleaning Information Storage.xlsx
+++ b/Data Cleaning Information Storage.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowanscassellati/Documents/GitHub/DSI-Hiatt-Visualizations/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953DCBC9-E6A1-F246-BE52-F70F1B9E44ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Semester Information" sheetId="1" r:id="rId1"/>
     <sheet name="Hiatt Staff Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Appointment Type Summation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Semester Name</t>
   </si>
@@ -33,6 +27,15 @@
     <t>End Date</t>
   </si>
   <si>
+    <t>This is a semester name that should get replaced</t>
+  </si>
+  <si>
+    <t>1/1/1111</t>
+  </si>
+  <si>
+    <t>9/9/9999</t>
+  </si>
+  <si>
     <t>Staff Emails</t>
   </si>
   <si>
@@ -82,19 +85,13 @@
   </si>
   <si>
     <t xml:space="preserve">Club Support </t>
-  </si>
-  <si>
-    <t>This is a semester name that should get replaced</t>
-  </si>
-  <si>
-    <t>Test 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,33 +143,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -210,7 +198,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -244,7 +232,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -279,10 +266,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -455,16 +441,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,26 +459,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2">
-        <v>46203</v>
-      </c>
-      <c r="C2" s="2">
-        <v>46203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2">
-        <v>46157</v>
-      </c>
-      <c r="C3" s="2">
-        <v>46157</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -503,46 +476,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -551,61 +524,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed for summer dataset
</commit_message>
<xml_diff>
--- a/Data Cleaning Information Storage.xlsx
+++ b/Data Cleaning Information Storage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Semester Name</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Appt Type Sum</t>
+  </si>
+  <si>
+    <t>Business Coach: 30-Minute Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health &amp; Science Coach: 30-Minute Meeting </t>
   </si>
   <si>
     <t>Law School Advisor: Extended Meeting</t>
@@ -525,7 +531,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -539,44 +545,54 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates from summer notes
</commit_message>
<xml_diff>
--- a/Data Cleaning Information Storage.xlsx
+++ b/Data Cleaning Information Storage.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Semester Information" sheetId="1" r:id="rId1"/>
     <sheet name="Hiatt Staff Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Appointment Type Summation" sheetId="3" r:id="rId3"/>
+    <sheet name="Event Type Name List" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Semester Name</t>
   </si>
@@ -91,6 +92,90 @@
   </si>
   <si>
     <t xml:space="preserve">Club Support </t>
+  </si>
+  <si>
+    <t>Event Type Name Accepted List</t>
+  </si>
+  <si>
+    <t>Appointment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big Interview </t>
+  </si>
+  <si>
+    <t>Career Closet</t>
+  </si>
+  <si>
+    <t>Career Course</t>
+  </si>
+  <si>
+    <t>Career Fair</t>
+  </si>
+  <si>
+    <t>Classroom Presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club Presentation </t>
+  </si>
+  <si>
+    <t>Completed Handshake Profile</t>
+  </si>
+  <si>
+    <t>Drop-In/Chat</t>
+  </si>
+  <si>
+    <t>Employer Partner Event</t>
+  </si>
+  <si>
+    <t>Employment Toolkit</t>
+  </si>
+  <si>
+    <t>Hiration</t>
+  </si>
+  <si>
+    <t>HS Employer Review</t>
+  </si>
+  <si>
+    <t>HS Interview Review</t>
+  </si>
+  <si>
+    <t>Info Session</t>
+  </si>
+  <si>
+    <t>Library Book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mentor Meetup </t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Possible Program (Fall Only?)</t>
+  </si>
+  <si>
+    <t>Project Onramp</t>
+  </si>
+  <si>
+    <t>Rise Together</t>
+  </si>
+  <si>
+    <t>Speaker/Panel</t>
+  </si>
+  <si>
+    <t>Trek</t>
+  </si>
+  <si>
+    <t>Type Focus</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
+    <t>WOW</t>
   </si>
 </sst>
 </file>
@@ -598,4 +683,162 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to incorporate Other checks
</commit_message>
<xml_diff>
--- a/Data Cleaning Information Storage.xlsx
+++ b/Data Cleaning Information Storage.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Hiatt Staff Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Appointment Type Summation" sheetId="3" r:id="rId3"/>
     <sheet name="Event Type Name List" sheetId="4" r:id="rId4"/>
+    <sheet name="Combined Name Type" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>Semester Name</t>
   </si>
@@ -176,6 +177,51 @@
   </si>
   <si>
     <t>WOW</t>
+  </si>
+  <si>
+    <t>Events Name</t>
+  </si>
+  <si>
+    <t>Event Type Name</t>
+  </si>
+  <si>
+    <t>Hiatt Library: Spring 2025</t>
+  </si>
+  <si>
+    <t>Possible Program: Spring 2025</t>
+  </si>
+  <si>
+    <t>Rise Together, Register Together</t>
+  </si>
+  <si>
+    <t>Moodle: Spring 2025</t>
+  </si>
+  <si>
+    <t>LinkedIn Photo Booth Pop-up (Sherman)</t>
+  </si>
+  <si>
+    <t>Career Closet: Spring 2025</t>
+  </si>
+  <si>
+    <t>TypeFocus: Spring 2025</t>
+  </si>
+  <si>
+    <t>Hiration: Spring 2025</t>
+  </si>
+  <si>
+    <t>HWL Applying to Law School: Spring 2025</t>
+  </si>
+  <si>
+    <t>INT 89: Spring 2025</t>
+  </si>
+  <si>
+    <t>Rise Together: Spring 2025</t>
+  </si>
+  <si>
+    <t>HWL Work, Career &amp; Life: Spring 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WOW: Spring 2025 </t>
   </si>
 </sst>
 </file>
@@ -841,4 +887,129 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>